<commit_message>
Daily attendance update - 2026-02-03
</commit_message>
<xml_diff>
--- a/data/App_Admin_UV-WCS.xlsx
+++ b/data/App_Admin_UV-WCS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\rethin\projects\wfo_tracker\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B57DB9-2B50-45A2-A22D-1C983CC8D43A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42279179-D771-45C9-A5E6-592F6E82F76C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="9" activeTab="11" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="10" activeTab="12" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
   </bookViews>
   <sheets>
     <sheet name="UV-WMS Admin Jan 2025" sheetId="9" r:id="rId1"/>
@@ -3486,7 +3486,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{988C623D-E1BD-4FE8-8DE5-A86BDEB0A522}">
   <dimension ref="A1:AJ17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+    <sheetView topLeftCell="L1" workbookViewId="0">
       <selection activeCell="AA3" sqref="AA3"/>
     </sheetView>
   </sheetViews>
@@ -4332,8 +4332,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9E71A27-DC0F-4421-B295-A887695B49EA}">
   <dimension ref="A1:AJ17"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="AE5" sqref="AE5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4585,8 +4585,8 @@
       <c r="F3" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>16</v>
+      <c r="G3" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
@@ -4926,8 +4926,8 @@
       <c r="AG6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="AH6" s="6" t="s">
-        <v>24</v>
+      <c r="AH6" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="AI6" s="5" t="s">
         <v>17</v>
@@ -4953,8 +4953,8 @@
       <c r="F7" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G7" s="4" t="s">
-        <v>16</v>
+      <c r="G7" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
@@ -5018,8 +5018,8 @@
       <c r="AG7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="AH7" s="5" t="s">
-        <v>17</v>
+      <c r="AH7" s="6" t="s">
+        <v>24</v>
       </c>
       <c r="AI7" s="5" t="s">
         <v>17</v>
@@ -5081,11 +5081,11 @@
       </c>
       <c r="B13" s="2">
         <f>COUNTIF(F3:AI3,"WFO")</f>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C13" s="2">
         <f>COUNTIF(F3:AI3,"WFH")</f>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:36" x14ac:dyDescent="0.25">
@@ -5124,7 +5124,7 @@
       </c>
       <c r="C16" s="2">
         <f>COUNTIF(F6:AI6,"WFH")</f>
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -5133,7 +5133,7 @@
       </c>
       <c r="B17" s="2">
         <f>COUNTIF(F7:AI7,"WFO")</f>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C17" s="2">
         <f>COUNTIF(F7:AI7,"WFH")</f>

</xml_diff>

<commit_message>
Daily attendance update - 2026-02-09
</commit_message>
<xml_diff>
--- a/data/App_Admin_UV-WCS.xlsx
+++ b/data/App_Admin_UV-WCS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\rethin\projects\wfo_tracker\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3F8F111-B8AD-495A-8899-DA70FE0D799F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B953D615-6718-45C0-8AC1-2B1D545BDF79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="8" activeTab="8" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="10" activeTab="13" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
   </bookViews>
   <sheets>
     <sheet name="UV-WMS Admin Jan 2025" sheetId="9" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2008" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2021" uniqueCount="29">
   <si>
     <t>Person</t>
   </si>
@@ -4749,8 +4749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F94C369-A483-4243-8B30-4AC8F8C2C920}">
   <dimension ref="A1:AG15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4987,9 +4987,15 @@
       <c r="H3" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
+      <c r="I3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="L3" s="7"/>
       <c r="M3" s="7"/>
       <c r="N3" s="2"/>
@@ -5036,12 +5042,20 @@
       <c r="H4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
+      <c r="I4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="L4" s="7"/>
       <c r="M4" s="7"/>
-      <c r="N4" s="2"/>
+      <c r="N4" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
@@ -5085,9 +5099,15 @@
       <c r="H5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
+      <c r="I5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="L5" s="7"/>
       <c r="M5" s="7"/>
       <c r="N5" s="2"/>
@@ -5134,9 +5154,15 @@
       <c r="H6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
+      <c r="I6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="L6" s="7"/>
       <c r="M6" s="7"/>
       <c r="N6" s="2"/>
@@ -5212,11 +5238,11 @@
       </c>
       <c r="B12" s="2">
         <f>COUNTIF(F3:AG3,"WFO")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C12" s="2">
         <f>COUNTIF(F3:AG3,"WFH")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.25">
@@ -5225,7 +5251,7 @@
       </c>
       <c r="B13" s="2">
         <f>COUNTIF(F4:AG4,"WFO")</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C13" s="2">
         <f>COUNTIF(F4:AG4,"WFH")</f>
@@ -5238,11 +5264,11 @@
       </c>
       <c r="B14" s="2">
         <f>COUNTIF(F5:AG5,"WFO")</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C14" s="2">
         <f>COUNTIF(F5:AG5,"WFH")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.25">
@@ -5255,7 +5281,7 @@
       </c>
       <c r="C15" s="2">
         <f>COUNTIF(F6:AG6,"WFH")</f>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -10345,8 +10371,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED7CEAED-F464-426C-A766-484A87191C7F}">
   <dimension ref="A1:AI15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:XFD15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Daily attendance update - 2026-02-11
</commit_message>
<xml_diff>
--- a/data/App_Admin_UV-WCS.xlsx
+++ b/data/App_Admin_UV-WCS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\rethin\projects\wfo_tracker\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B953D615-6718-45C0-8AC1-2B1D545BDF79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A3B2147-DB49-45DE-B11F-FE01975B24F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="10" activeTab="13" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="10" activeTab="13" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
   </bookViews>
   <sheets>
     <sheet name="UV-WMS Admin Jan 2025" sheetId="9" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2021" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2032" uniqueCount="29">
   <si>
     <t>Person</t>
   </si>
@@ -4750,7 +4750,7 @@
   <dimension ref="A1:AG15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="P3" sqref="P3:P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4998,9 +4998,15 @@
       </c>
       <c r="L3" s="7"/>
       <c r="M3" s="7"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
+      <c r="N3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="O3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
       <c r="S3" s="7"/>
@@ -5056,8 +5062,12 @@
       <c r="N4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
+      <c r="O4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="P4" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="Q4" s="2"/>
       <c r="R4" s="2"/>
       <c r="S4" s="7"/>
@@ -5110,9 +5120,15 @@
       </c>
       <c r="L5" s="7"/>
       <c r="M5" s="7"/>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
-      <c r="P5" s="2"/>
+      <c r="N5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="O5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="P5" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
       <c r="S5" s="7"/>
@@ -5165,9 +5181,15 @@
       </c>
       <c r="L6" s="7"/>
       <c r="M6" s="7"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
+      <c r="N6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="O6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="P6" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="Q6" s="2"/>
       <c r="R6" s="2"/>
       <c r="S6" s="7"/>
@@ -5238,11 +5260,11 @@
       </c>
       <c r="B12" s="2">
         <f>COUNTIF(F3:AG3,"WFO")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C12" s="2">
         <f>COUNTIF(F3:AG3,"WFH")</f>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.25">
@@ -5255,7 +5277,7 @@
       </c>
       <c r="C13" s="2">
         <f>COUNTIF(F4:AG4,"WFH")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.25">
@@ -5264,11 +5286,11 @@
       </c>
       <c r="B14" s="2">
         <f>COUNTIF(F5:AG5,"WFO")</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C14" s="2">
         <f>COUNTIF(F5:AG5,"WFH")</f>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.25">
@@ -5281,7 +5303,7 @@
       </c>
       <c r="C15" s="2">
         <f>COUNTIF(F6:AG6,"WFH")</f>
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daily attendance update - 2026-02-12
</commit_message>
<xml_diff>
--- a/data/App_Admin_UV-WCS.xlsx
+++ b/data/App_Admin_UV-WCS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\rethin\projects\wfo_tracker\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A3B2147-DB49-45DE-B11F-FE01975B24F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E385D595-93C6-404C-A1DA-A3A96F5810C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="10" activeTab="13" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="10" activeTab="13" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
   </bookViews>
   <sheets>
     <sheet name="UV-WMS Admin Jan 2025" sheetId="9" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2032" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2040" uniqueCount="29">
   <si>
     <t>Person</t>
   </si>
@@ -4750,7 +4750,7 @@
   <dimension ref="A1:AG15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3:P6"/>
+      <selection activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5007,8 +5007,12 @@
       <c r="P3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
+      <c r="Q3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="R3" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="S3" s="7"/>
       <c r="T3" s="7"/>
       <c r="U3" s="2"/>
@@ -5068,8 +5072,12 @@
       <c r="P4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
+      <c r="Q4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="R4" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="S4" s="7"/>
       <c r="T4" s="7"/>
       <c r="U4" s="2"/>
@@ -5129,8 +5137,12 @@
       <c r="P5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="Q5" s="2"/>
-      <c r="R5" s="2"/>
+      <c r="Q5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="R5" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="S5" s="7"/>
       <c r="T5" s="7"/>
       <c r="U5" s="2"/>
@@ -5190,8 +5202,12 @@
       <c r="P6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="Q6" s="2"/>
-      <c r="R6" s="2"/>
+      <c r="Q6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="R6" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="S6" s="7"/>
       <c r="T6" s="7"/>
       <c r="U6" s="2"/>
@@ -5264,7 +5280,7 @@
       </c>
       <c r="C12" s="2">
         <f>COUNTIF(F3:AG3,"WFH")</f>
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.25">
@@ -5273,7 +5289,7 @@
       </c>
       <c r="B13" s="2">
         <f>COUNTIF(F4:AG4,"WFO")</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C13" s="2">
         <f>COUNTIF(F4:AG4,"WFH")</f>
@@ -5286,11 +5302,11 @@
       </c>
       <c r="B14" s="2">
         <f>COUNTIF(F5:AG5,"WFO")</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C14" s="2">
         <f>COUNTIF(F5:AG5,"WFH")</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.25">
@@ -5303,7 +5319,7 @@
       </c>
       <c r="C15" s="2">
         <f>COUNTIF(F6:AG6,"WFH")</f>
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daily attendance update - 2026-02-16
</commit_message>
<xml_diff>
--- a/data/App_Admin_UV-WCS.xlsx
+++ b/data/App_Admin_UV-WCS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\rethin\projects\wfo_tracker\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E385D595-93C6-404C-A1DA-A3A96F5810C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE970214-AE61-456D-85B8-F740B31F1070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="10" activeTab="13" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="10" activeTab="13" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
   </bookViews>
   <sheets>
     <sheet name="UV-WMS Admin Jan 2025" sheetId="9" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2040" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2044" uniqueCount="29">
   <si>
     <t>Person</t>
   </si>
@@ -1037,31 +1037,31 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="23" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="25" max="30" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="32" max="33" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="35" max="36" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="18" max="23" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="25" max="30" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="32" max="33" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="35" max="36" width="9.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -1171,7 +1171,7 @@
         <v>45688</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -1271,7 +1271,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -1365,7 +1365,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -1459,7 +1459,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -1553,7 +1553,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -1647,7 +1647,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -1741,7 +1741,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
         <v>1</v>
       </c>
@@ -1752,7 +1752,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
@@ -1765,7 +1765,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
@@ -1778,7 +1778,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>20</v>
       </c>
@@ -1791,7 +1791,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>22</v>
       </c>
@@ -1804,7 +1804,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>23</v>
       </c>
@@ -1838,30 +1838,30 @@
       <selection activeCell="A15" sqref="A15:XFD15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="12" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="19" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="24" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="28" max="33" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="35" max="36" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="12" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="15" max="19" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="21" max="24" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="28" max="33" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="35" max="36" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -1971,7 +1971,7 @@
         <v>45961</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -2071,7 +2071,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -2165,7 +2165,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -2259,7 +2259,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -2353,7 +2353,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>23</v>
       </c>
@@ -2447,7 +2447,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -2485,7 +2485,7 @@
       <c r="AI7" s="2"/>
       <c r="AJ7" s="2"/>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
         <v>1</v>
       </c>
@@ -2496,7 +2496,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
@@ -2509,7 +2509,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>19</v>
       </c>
@@ -2522,7 +2522,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
@@ -2535,7 +2535,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>23</v>
       </c>
@@ -2580,26 +2580,26 @@
       <selection activeCell="A15" sqref="A15:XFD15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="14" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="23" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="25" max="30" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="32" max="35" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="14" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="18" max="23" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="25" max="30" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="32" max="35" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -2706,7 +2706,7 @@
         <v>45991</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -2803,7 +2803,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -2890,7 +2890,7 @@
       <c r="AH3" s="7"/>
       <c r="AI3" s="7"/>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -2977,7 +2977,7 @@
       <c r="AH4" s="7"/>
       <c r="AI4" s="7"/>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -3064,7 +3064,7 @@
       <c r="AH5" s="7"/>
       <c r="AI5" s="7"/>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>23</v>
       </c>
@@ -3151,7 +3151,7 @@
       <c r="AH6" s="7"/>
       <c r="AI6" s="7"/>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -3188,7 +3188,7 @@
       <c r="AH7" s="2"/>
       <c r="AI7" s="2"/>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
         <v>1</v>
       </c>
@@ -3199,7 +3199,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
@@ -3212,7 +3212,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>19</v>
       </c>
@@ -3225,7 +3225,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
@@ -3238,7 +3238,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>23</v>
       </c>
@@ -3283,27 +3283,27 @@
       <selection activeCell="A15" sqref="A15:XFD15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="14" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="23" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="25" max="30" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="32" max="35" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="14" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="18" max="23" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="25" max="30" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="32" max="35" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="11.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -3413,7 +3413,7 @@
         <v>46022</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -3513,7 +3513,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -3607,7 +3607,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -3701,7 +3701,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -3795,7 +3795,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>23</v>
       </c>
@@ -3889,7 +3889,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -3927,7 +3927,7 @@
       <c r="AI7" s="2"/>
       <c r="AJ7" s="2"/>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
         <v>1</v>
       </c>
@@ -3938,7 +3938,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
@@ -3951,7 +3951,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>19</v>
       </c>
@@ -3964,7 +3964,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
@@ -3977,7 +3977,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>23</v>
       </c>
@@ -4022,27 +4022,27 @@
       <selection activeCell="V28" sqref="V28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="14" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="23" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="25" max="30" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="32" max="35" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="14" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="18" max="23" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="25" max="30" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="32" max="35" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="11.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -4152,7 +4152,7 @@
         <v>46053</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -4252,7 +4252,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -4344,7 +4344,7 @@
       </c>
       <c r="AJ3" s="7"/>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -4436,7 +4436,7 @@
       </c>
       <c r="AJ4" s="7"/>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -4528,7 +4528,7 @@
       </c>
       <c r="AJ5" s="7"/>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>23</v>
       </c>
@@ -4620,7 +4620,7 @@
       </c>
       <c r="AJ6" s="7"/>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -4658,7 +4658,7 @@
       <c r="AI7" s="2"/>
       <c r="AJ7" s="2"/>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
         <v>1</v>
       </c>
@@ -4669,7 +4669,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
@@ -4682,7 +4682,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>19</v>
       </c>
@@ -4695,7 +4695,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
@@ -4708,7 +4708,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>23</v>
       </c>
@@ -4749,30 +4749,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F94C369-A483-4243-8B30-4AC8F8C2C920}">
   <dimension ref="A1:AG15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R6" sqref="R6"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="U4" sqref="U4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="14" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="23" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="25" max="30" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="32" max="33" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="14" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="18" max="23" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="25" max="30" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="32" max="33" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -4873,7 +4873,7 @@
         <v>46081</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -4964,7 +4964,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -5015,7 +5015,9 @@
       </c>
       <c r="S3" s="7"/>
       <c r="T3" s="7"/>
-      <c r="U3" s="2"/>
+      <c r="U3" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="V3" s="2"/>
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
@@ -5029,7 +5031,7 @@
       <c r="AF3" s="2"/>
       <c r="AG3" s="7"/>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -5080,7 +5082,9 @@
       </c>
       <c r="S4" s="7"/>
       <c r="T4" s="7"/>
-      <c r="U4" s="2"/>
+      <c r="U4" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="V4" s="2"/>
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
@@ -5094,7 +5098,7 @@
       <c r="AF4" s="2"/>
       <c r="AG4" s="7"/>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -5145,7 +5149,9 @@
       </c>
       <c r="S5" s="7"/>
       <c r="T5" s="7"/>
-      <c r="U5" s="2"/>
+      <c r="U5" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="V5" s="2"/>
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
@@ -5159,7 +5165,7 @@
       <c r="AF5" s="2"/>
       <c r="AG5" s="7"/>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>23</v>
       </c>
@@ -5210,7 +5216,9 @@
       </c>
       <c r="S6" s="7"/>
       <c r="T6" s="7"/>
-      <c r="U6" s="2"/>
+      <c r="U6" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="V6" s="2"/>
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
@@ -5224,7 +5232,7 @@
       <c r="AF6" s="2"/>
       <c r="AG6" s="7"/>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -5259,7 +5267,7 @@
       <c r="AF7" s="2"/>
       <c r="AG7" s="2"/>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
         <v>1</v>
       </c>
@@ -5270,20 +5278,20 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="2">
         <f>COUNTIF(F3:AG3,"WFO")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C12" s="2">
         <f>COUNTIF(F3:AG3,"WFH")</f>
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>19</v>
       </c>
@@ -5293,10 +5301,10 @@
       </c>
       <c r="C13" s="2">
         <f>COUNTIF(F4:AG4,"WFH")</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
@@ -5306,10 +5314,10 @@
       </c>
       <c r="C14" s="2">
         <f>COUNTIF(F5:AG5,"WFH")</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>23</v>
       </c>
@@ -5319,7 +5327,7 @@
       </c>
       <c r="C15" s="2">
         <f>COUNTIF(F6:AG6,"WFH")</f>
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -5355,30 +5363,30 @@
       <selection activeCell="AC6" sqref="AC6:AG6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="23" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="25" max="30" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="32" max="33" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="18" max="23" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="25" max="30" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="32" max="33" width="9.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -5479,7 +5487,7 @@
         <v>45716</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -5570,7 +5578,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -5655,7 +5663,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -5742,7 +5750,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -5829,7 +5837,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -5914,7 +5922,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -5999,7 +6007,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
         <v>1</v>
       </c>
@@ -6010,7 +6018,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
@@ -6023,7 +6031,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
@@ -6036,7 +6044,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>20</v>
       </c>
@@ -6049,7 +6057,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>22</v>
       </c>
@@ -6062,7 +6070,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>23</v>
       </c>
@@ -6097,28 +6105,28 @@
       <selection pane="topRight" activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.26953125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="8.81640625" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="10" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.26953125" bestFit="1" customWidth="1"/>
     <col min="18" max="23" width="10" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.26953125" bestFit="1" customWidth="1"/>
     <col min="25" max="30" width="10" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.26953125" bestFit="1" customWidth="1"/>
     <col min="32" max="35" width="10" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="10.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -6228,7 +6236,7 @@
         <v>45747</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -6328,7 +6336,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -6418,7 +6426,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -6506,7 +6514,7 @@
       <c r="AI4" s="2"/>
       <c r="AJ4" s="13"/>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -6594,7 +6602,7 @@
       <c r="AI5" s="2"/>
       <c r="AJ5" s="13"/>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>23</v>
       </c>
@@ -6682,7 +6690,7 @@
       <c r="AI6" s="2"/>
       <c r="AJ6" s="13"/>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -6720,7 +6728,7 @@
       <c r="AI7" s="2"/>
       <c r="AJ7" s="14"/>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A9" s="8" t="s">
         <v>1</v>
       </c>
@@ -6731,7 +6739,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
@@ -6744,7 +6752,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>19</v>
       </c>
@@ -6757,7 +6765,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>20</v>
       </c>
@@ -6770,7 +6778,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>23</v>
       </c>
@@ -6814,29 +6822,29 @@
       <selection pane="topRight" activeCell="A14" sqref="A14:XFD14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.26953125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="8.81640625" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="10" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.26953125" bestFit="1" customWidth="1"/>
     <col min="18" max="23" width="10" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.26953125" bestFit="1" customWidth="1"/>
     <col min="25" max="30" width="10" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.26953125" bestFit="1" customWidth="1"/>
     <col min="32" max="35" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -6943,7 +6951,7 @@
         <v>45777</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -7040,7 +7048,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -7131,7 +7139,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -7222,7 +7230,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -7313,7 +7321,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>23</v>
       </c>
@@ -7404,7 +7412,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -7441,7 +7449,7 @@
       <c r="AH7" s="2"/>
       <c r="AI7" s="2"/>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
         <v>1</v>
       </c>
@@ -7452,7 +7460,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
@@ -7465,7 +7473,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
@@ -7478,7 +7486,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>20</v>
       </c>
@@ -7491,7 +7499,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>23</v>
       </c>
@@ -7535,29 +7543,29 @@
       <selection pane="topRight" activeCell="A14" sqref="A14:XFD14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="18" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="25" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="27" max="32" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="34" max="36" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="15" max="18" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="20" max="25" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="27" max="32" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="34" max="36" width="9.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -7667,7 +7675,7 @@
         <v>45808</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -7767,7 +7775,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -7859,7 +7867,7 @@
       </c>
       <c r="AJ3" s="7"/>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -7951,7 +7959,7 @@
       </c>
       <c r="AJ4" s="7"/>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -8043,7 +8051,7 @@
       </c>
       <c r="AJ5" s="7"/>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>23</v>
       </c>
@@ -8135,7 +8143,7 @@
       </c>
       <c r="AJ6" s="7"/>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -8172,7 +8180,7 @@
       <c r="AH7" s="2"/>
       <c r="AI7" s="2"/>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
         <v>1</v>
       </c>
@@ -8183,7 +8191,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
@@ -8196,7 +8204,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
@@ -8209,7 +8217,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>20</v>
       </c>
@@ -8222,7 +8230,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>23</v>
       </c>
@@ -8270,15 +8278,15 @@
       <selection pane="topRight" activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -8385,7 +8393,7 @@
         <v>45838</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -8482,7 +8490,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -8571,7 +8579,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -8660,7 +8668,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -8749,7 +8757,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>23</v>
       </c>
@@ -8838,7 +8846,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -8875,7 +8883,7 @@
       <c r="AH7" s="2"/>
       <c r="AI7" s="2"/>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="s">
         <v>1</v>
       </c>
@@ -8886,7 +8894,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
@@ -8899,7 +8907,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>19</v>
       </c>
@@ -8912,7 +8920,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
@@ -8925,7 +8933,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>23</v>
       </c>
@@ -8970,17 +8978,17 @@
       <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -9090,7 +9098,7 @@
         <v>45869</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -9190,7 +9198,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -9284,7 +9292,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -9378,7 +9386,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -9472,7 +9480,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>23</v>
       </c>
@@ -9566,7 +9574,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -9603,7 +9611,7 @@
       <c r="AH7" s="2"/>
       <c r="AI7" s="2"/>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
         <v>1</v>
       </c>
@@ -9614,7 +9622,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
@@ -9627,7 +9635,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>19</v>
       </c>
@@ -9640,7 +9648,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
@@ -9653,7 +9661,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>23</v>
       </c>
@@ -9698,18 +9706,18 @@
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -9820,7 +9828,7 @@
       </c>
       <c r="AK1" s="1"/>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -9920,7 +9928,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -10010,7 +10018,7 @@
       <c r="AI3" s="7"/>
       <c r="AJ3" s="7"/>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -10100,7 +10108,7 @@
       <c r="AI4" s="7"/>
       <c r="AJ4" s="7"/>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -10190,7 +10198,7 @@
       <c r="AI5" s="7"/>
       <c r="AJ5" s="7"/>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>23</v>
       </c>
@@ -10280,7 +10288,7 @@
       <c r="AI6" s="7"/>
       <c r="AJ6" s="7"/>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -10318,7 +10326,7 @@
       <c r="AI7" s="2"/>
       <c r="AJ7" s="2"/>
     </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
         <v>1</v>
       </c>
@@ -10329,7 +10337,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
@@ -10342,7 +10350,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>19</v>
       </c>
@@ -10355,7 +10363,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
@@ -10368,7 +10376,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>23</v>
       </c>
@@ -10413,19 +10421,19 @@
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -10532,7 +10540,7 @@
         <v>45930</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -10629,7 +10637,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -10720,7 +10728,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -10811,7 +10819,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -10902,7 +10910,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>23</v>
       </c>
@@ -10993,7 +11001,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -11030,7 +11038,7 @@
       <c r="AH7" s="2"/>
       <c r="AI7" s="2"/>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
         <v>1</v>
       </c>
@@ -11041,7 +11049,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
@@ -11054,7 +11062,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>19</v>
       </c>
@@ -11067,7 +11075,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
@@ -11080,7 +11088,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
Daily attendance update - 2026-02-20
</commit_message>
<xml_diff>
--- a/data/App_Admin_UV-WCS.xlsx
+++ b/data/App_Admin_UV-WCS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\rethin\projects\wfo_tracker\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE970214-AE61-456D-85B8-F740B31F1070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7A64977-1006-4BF1-901D-28D16FB85DBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="10" activeTab="13" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
   </bookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2044" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2060" uniqueCount="29">
   <si>
     <t>Person</t>
   </si>
@@ -4749,8 +4749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F94C369-A483-4243-8B30-4AC8F8C2C920}">
   <dimension ref="A1:AG15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="U4" sqref="U4"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="X5" sqref="X5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5018,10 +5018,18 @@
       <c r="U3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="V3" s="2"/>
-      <c r="W3" s="2"/>
-      <c r="X3" s="2"/>
-      <c r="Y3" s="2"/>
+      <c r="V3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="W3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="X3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y3" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="Z3" s="7"/>
       <c r="AA3" s="7"/>
       <c r="AB3" s="2"/>
@@ -5085,10 +5093,18 @@
       <c r="U4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="V4" s="2"/>
-      <c r="W4" s="2"/>
-      <c r="X4" s="2"/>
-      <c r="Y4" s="2"/>
+      <c r="V4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="W4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="X4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y4" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="Z4" s="7"/>
       <c r="AA4" s="7"/>
       <c r="AB4" s="2"/>
@@ -5152,10 +5168,18 @@
       <c r="U5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="V5" s="2"/>
-      <c r="W5" s="2"/>
-      <c r="X5" s="2"/>
-      <c r="Y5" s="2"/>
+      <c r="V5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="W5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="X5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y5" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="Z5" s="7"/>
       <c r="AA5" s="7"/>
       <c r="AB5" s="2"/>
@@ -5219,10 +5243,18 @@
       <c r="U6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="V6" s="2"/>
-      <c r="W6" s="2"/>
-      <c r="X6" s="2"/>
-      <c r="Y6" s="2"/>
+      <c r="V6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="W6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="X6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y6" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="Z6" s="7"/>
       <c r="AA6" s="7"/>
       <c r="AB6" s="2"/>
@@ -5284,11 +5316,11 @@
       </c>
       <c r="B12" s="2">
         <f>COUNTIF(F3:AG3,"WFO")</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C12" s="2">
         <f>COUNTIF(F3:AG3,"WFH")</f>
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.35">
@@ -5301,7 +5333,7 @@
       </c>
       <c r="C13" s="2">
         <f>COUNTIF(F4:AG4,"WFH")</f>
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.35">
@@ -5310,11 +5342,11 @@
       </c>
       <c r="B14" s="2">
         <f>COUNTIF(F5:AG5,"WFO")</f>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C14" s="2">
         <f>COUNTIF(F5:AG5,"WFH")</f>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.35">
@@ -5327,7 +5359,7 @@
       </c>
       <c r="C15" s="2">
         <f>COUNTIF(F6:AG6,"WFH")</f>
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daily attendance update - 2026-02-25
</commit_message>
<xml_diff>
--- a/data/App_Admin_UV-WCS.xlsx
+++ b/data/App_Admin_UV-WCS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\rethin\projects\wfo_tracker\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7A64977-1006-4BF1-901D-28D16FB85DBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01433FD0-7FD9-4A5D-AB47-B940322C87F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="10" activeTab="13" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
   </bookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2060" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2074" uniqueCount="29">
   <si>
     <t>Person</t>
   </si>
@@ -4749,8 +4749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F94C369-A483-4243-8B30-4AC8F8C2C920}">
   <dimension ref="A1:AG15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="X5" sqref="X5"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="AE7" sqref="AE7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5032,9 +5032,15 @@
       </c>
       <c r="Z3" s="7"/>
       <c r="AA3" s="7"/>
-      <c r="AB3" s="2"/>
-      <c r="AC3" s="2"/>
-      <c r="AD3" s="2"/>
+      <c r="AB3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AC3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD3" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="AE3" s="2"/>
       <c r="AF3" s="2"/>
       <c r="AG3" s="7"/>
@@ -5107,11 +5113,21 @@
       </c>
       <c r="Z4" s="7"/>
       <c r="AA4" s="7"/>
-      <c r="AB4" s="2"/>
-      <c r="AC4" s="2"/>
-      <c r="AD4" s="2"/>
-      <c r="AE4" s="2"/>
-      <c r="AF4" s="2"/>
+      <c r="AB4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AE4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AF4" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="AG4" s="7"/>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.35">
@@ -5182,9 +5198,15 @@
       </c>
       <c r="Z5" s="7"/>
       <c r="AA5" s="7"/>
-      <c r="AB5" s="2"/>
-      <c r="AC5" s="2"/>
-      <c r="AD5" s="2"/>
+      <c r="AB5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AC5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AD5" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="AE5" s="2"/>
       <c r="AF5" s="2"/>
       <c r="AG5" s="7"/>
@@ -5257,9 +5279,15 @@
       </c>
       <c r="Z6" s="7"/>
       <c r="AA6" s="7"/>
-      <c r="AB6" s="2"/>
-      <c r="AC6" s="2"/>
-      <c r="AD6" s="2"/>
+      <c r="AB6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AC6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AD6" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="AE6" s="2"/>
       <c r="AF6" s="2"/>
       <c r="AG6" s="7"/>
@@ -5316,11 +5344,11 @@
       </c>
       <c r="B12" s="2">
         <f>COUNTIF(F3:AG3,"WFO")</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C12" s="2">
         <f>COUNTIF(F3:AG3,"WFH")</f>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.35">
@@ -5333,7 +5361,7 @@
       </c>
       <c r="C13" s="2">
         <f>COUNTIF(F4:AG4,"WFH")</f>
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.35">
@@ -5342,11 +5370,11 @@
       </c>
       <c r="B14" s="2">
         <f>COUNTIF(F5:AG5,"WFO")</f>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C14" s="2">
         <f>COUNTIF(F5:AG5,"WFH")</f>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.35">
@@ -5355,7 +5383,7 @@
       </c>
       <c r="B15" s="2">
         <f>COUNTIF(F6:AG6,"WFO")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C15" s="2">
         <f>COUNTIF(F6:AG6,"WFH")</f>

</xml_diff>

<commit_message>
Daily attendance update - 2026-02-26
</commit_message>
<xml_diff>
--- a/data/App_Admin_UV-WCS.xlsx
+++ b/data/App_Admin_UV-WCS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\rethin\projects\wfo_tracker\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01433FD0-7FD9-4A5D-AB47-B940322C87F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB00E355-7091-4BE3-AE1E-45A2248D5BB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="10" activeTab="13" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
   </bookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2074" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2077" uniqueCount="29">
   <si>
     <t>Person</t>
   </si>
@@ -4750,7 +4750,7 @@
   <dimension ref="A1:AG15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="AE7" sqref="AE7"/>
+      <selection activeCell="AE3" sqref="AE3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5041,7 +5041,9 @@
       <c r="AD3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="AE3" s="2"/>
+      <c r="AE3" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="AF3" s="2"/>
       <c r="AG3" s="7"/>
     </row>
@@ -5207,7 +5209,9 @@
       <c r="AD5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="AE5" s="2"/>
+      <c r="AE5" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="AF5" s="2"/>
       <c r="AG5" s="7"/>
     </row>
@@ -5288,7 +5292,9 @@
       <c r="AD6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="AE6" s="2"/>
+      <c r="AE6" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="AF6" s="2"/>
       <c r="AG6" s="7"/>
     </row>
@@ -5348,7 +5354,7 @@
       </c>
       <c r="C12" s="2">
         <f>COUNTIF(F3:AG3,"WFH")</f>
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.35">
@@ -5370,7 +5376,7 @@
       </c>
       <c r="B14" s="2">
         <f>COUNTIF(F5:AG5,"WFO")</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C14" s="2">
         <f>COUNTIF(F5:AG5,"WFH")</f>
@@ -5387,7 +5393,7 @@
       </c>
       <c r="C15" s="2">
         <f>COUNTIF(F6:AG6,"WFH")</f>
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daily attendance update - 2026-02-27
</commit_message>
<xml_diff>
--- a/data/App_Admin_UV-WCS.xlsx
+++ b/data/App_Admin_UV-WCS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\rethin\projects\wfo_tracker\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB00E355-7091-4BE3-AE1E-45A2248D5BB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D7EBD9B-4054-451E-A0B6-167931150A48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="10" activeTab="13" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
   </bookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2077" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2080" uniqueCount="29">
   <si>
     <t>Person</t>
   </si>
@@ -4750,7 +4750,7 @@
   <dimension ref="A1:AG15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="AE3" sqref="AE3"/>
+      <selection activeCell="AF3" sqref="AF3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5044,7 +5044,9 @@
       <c r="AE3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="AF3" s="2"/>
+      <c r="AF3" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="AG3" s="7"/>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.35">
@@ -5212,7 +5214,9 @@
       <c r="AE5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="AF5" s="2"/>
+      <c r="AF5" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="AG5" s="7"/>
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.35">
@@ -5295,7 +5299,9 @@
       <c r="AE6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="AF6" s="2"/>
+      <c r="AF6" s="6" t="s">
+        <v>18</v>
+      </c>
       <c r="AG6" s="7"/>
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.35">
@@ -5354,7 +5360,7 @@
       </c>
       <c r="C12" s="2">
         <f>COUNTIF(F3:AG3,"WFH")</f>
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.35">
@@ -5380,7 +5386,7 @@
       </c>
       <c r="C14" s="2">
         <f>COUNTIF(F5:AG5,"WFH")</f>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.35">

</xml_diff>